<commit_message>
Edited the driver stats a bit to be more realistic
</commit_message>
<xml_diff>
--- a/Docs/DriverStats.xlsx
+++ b/Docs/DriverStats.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\A2B-Project\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -11,7 +16,10 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$B$2:$H$32</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -132,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,6 +238,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -277,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -310,9 +321,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,6 +373,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -524,18 +569,18 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
@@ -563,27 +608,27 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4">
         <f>ROUND(AVERAGE(D3:F3),1)</f>
-        <v>95.3</v>
+        <v>96</v>
       </c>
       <c r="H3" s="4">
         <f>(ROUND((G3/1.5)*1000000,-5))/1000000</f>
-        <v>63.5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -597,493 +642,493 @@
         <v>97</v>
       </c>
       <c r="E4" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F4" s="4">
         <v>93</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G32" si="0">ROUND(AVERAGE(D4:F4),1)</f>
-        <v>94.7</v>
+        <f>ROUND(AVERAGE(D4:F4),1)</f>
+        <v>95</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H32" si="1">(ROUND((G4/1.5)*1000000,-5))/1000000</f>
-        <v>63.1</v>
+        <f>(ROUND((G4/1.5)*1000000,-5))/1000000</f>
+        <v>63.3</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E5" s="4">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="4">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D5:F5),1)</f>
         <v>94.7</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G5/1.5)*1000000,-5))/1000000</f>
         <v>63.1</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E6" s="4">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F6" s="4">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
-        <v>85.7</v>
+        <f>ROUND(AVERAGE(D6:F6),1)</f>
+        <v>94</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>57.1</v>
+        <f>(ROUND((G6/1.5)*1000000,-5))/1000000</f>
+        <v>62.7</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E7" s="4">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="F7" s="4">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" si="0"/>
-        <v>77.3</v>
+        <f>ROUND(AVERAGE(D7:F7),1)</f>
+        <v>92.3</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>51.5</v>
+        <f>(ROUND((G7/1.5)*1000000,-5))/1000000</f>
+        <v>61.5</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E8" s="4">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F8" s="4">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>83</v>
+        <f>ROUND(AVERAGE(D8:F8),1)</f>
+        <v>90.7</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="1"/>
-        <v>55.3</v>
+        <f>(ROUND((G8/1.5)*1000000,-5))/1000000</f>
+        <v>60.5</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E9" s="4">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4">
         <v>85</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" si="0"/>
-        <v>88.7</v>
+        <f>ROUND(AVERAGE(D9:F9),1)</f>
+        <v>85.7</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>59.1</v>
+        <f>(ROUND((G9/1.5)*1000000,-5))/1000000</f>
+        <v>57.1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E10" s="4">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F10" s="4">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>96.7</v>
+        <f>ROUND(AVERAGE(D10:F10),1)</f>
+        <v>84</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>64.5</v>
+        <f>(ROUND((G10/1.5)*1000000,-5))/1000000</f>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D11" s="4">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F11" s="4">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="0"/>
-        <v>78.3</v>
+        <f>ROUND(AVERAGE(D11:F11),1)</f>
+        <v>82.3</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>52.2</v>
+        <f>(ROUND((G11/1.5)*1000000,-5))/1000000</f>
+        <v>54.9</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E12" s="4">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F12" s="4">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="0"/>
-        <v>83.3</v>
+        <f>ROUND(AVERAGE(D12:F12),1)</f>
+        <v>79.7</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>55.5</v>
+        <f>(ROUND((G12/1.5)*1000000,-5))/1000000</f>
+        <v>53.1</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D13" s="4">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E13" s="4">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F13" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>80.3</v>
+        <f>ROUND(AVERAGE(D13:F13),1)</f>
+        <v>78.7</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>53.5</v>
+        <f>(ROUND((G13/1.5)*1000000,-5))/1000000</f>
+        <v>52.5</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F14" s="4">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <f>ROUND(AVERAGE(D14:F14),1)</f>
+        <v>78.7</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f>(ROUND((G14/1.5)*1000000,-5))/1000000</f>
+        <v>52.5</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C15" s="5">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F15" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>74</v>
+        <f>ROUND(AVERAGE(D15:F15),1)</f>
+        <v>77.3</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>49.3</v>
+        <f>(ROUND((G15/1.5)*1000000,-5))/1000000</f>
+        <v>51.5</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
+        <v>78</v>
+      </c>
+      <c r="E16" s="4">
+        <v>73</v>
+      </c>
+      <c r="F16" s="4">
         <v>80</v>
       </c>
-      <c r="E16" s="4">
-        <v>74</v>
-      </c>
-      <c r="F16" s="4">
-        <v>73</v>
-      </c>
       <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>75.7</v>
+        <f>ROUND(AVERAGE(D16:F16),1)</f>
+        <v>77</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>50.5</v>
+        <f>(ROUND((G16/1.5)*1000000,-5))/1000000</f>
+        <v>51.3</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C17" s="5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D17" s="4">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F17" s="4">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>ROUND(AVERAGE(D17:F17),1)</f>
+        <v>77</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f>(ROUND((G17/1.5)*1000000,-5))/1000000</f>
+        <v>51.3</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C18" s="5">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E18" s="4">
         <v>76</v>
       </c>
       <c r="F18" s="4">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="0"/>
-        <v>76.3</v>
+        <f>ROUND(AVERAGE(D18:F18),1)</f>
+        <v>76.7</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="1"/>
-        <v>50.9</v>
+        <f>(ROUND((G18/1.5)*1000000,-5))/1000000</f>
+        <v>51.1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D19" s="4">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E19" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F19" s="4">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="0"/>
-        <v>76.3</v>
+        <f>ROUND(AVERAGE(D19:F19),1)</f>
+        <v>75</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>50.9</v>
+        <f>(ROUND((G19/1.5)*1000000,-5))/1000000</f>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D20" s="4">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E20" s="4">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F20" s="4">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D20:F20),1)</f>
         <v>75</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G20/1.5)*1000000,-5))/1000000</f>
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E21" s="4">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4">
         <v>74</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>ROUND(AVERAGE(D21:F21),1)</f>
+        <v>74</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f>(ROUND((G21/1.5)*1000000,-5))/1000000</f>
+        <v>49.3</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4">
+        <v>73</v>
+      </c>
+      <c r="E22" s="4">
+        <v>72</v>
+      </c>
+      <c r="F22" s="4">
         <v>71</v>
       </c>
-      <c r="E22" s="4">
-        <v>70</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
+        <f>ROUND(AVERAGE(D22:F22),1)</f>
         <v>72</v>
       </c>
-      <c r="G22" s="4">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
       <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>47.3</v>
+        <f>(ROUND((G22/1.5)*1000000,-5))/1000000</f>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="5">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D23" s="4">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E23" s="4">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F23" s="4">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="0"/>
-        <v>76.7</v>
+        <f>ROUND(AVERAGE(D23:F23),1)</f>
+        <v>71</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>51.1</v>
+        <f>(ROUND((G23/1.5)*1000000,-5))/1000000</f>
+        <v>47.3</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1103,11 +1148,11 @@
         <v>69</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D24:F24),1)</f>
         <v>70</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G24/1.5)*1000000,-5))/1000000</f>
         <v>46.7</v>
       </c>
     </row>
@@ -1128,37 +1173,37 @@
         <v>66</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D25:F25),1)</f>
         <v>69.3</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G25/1.5)*1000000,-5))/1000000</f>
         <v>46.2</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E26" s="4">
+        <v>67</v>
+      </c>
+      <c r="F26" s="4">
         <v>65</v>
       </c>
-      <c r="F26" s="4">
-        <v>63</v>
-      </c>
       <c r="G26" s="4">
-        <f t="shared" si="0"/>
-        <v>65.7</v>
+        <f>ROUND(AVERAGE(D26:F26),1)</f>
+        <v>68</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>43.8</v>
+        <f>(ROUND((G26/1.5)*1000000,-5))/1000000</f>
+        <v>45.3</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1178,87 +1223,87 @@
         <v>64</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D27:F27),1)</f>
         <v>67</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G27/1.5)*1000000,-5))/1000000</f>
         <v>44.7</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D28" s="4">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E28" s="4">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F28" s="4">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>ROUND(AVERAGE(D28:F28),1)</f>
+        <v>66</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="1"/>
-        <v>45.3</v>
+        <f>(ROUND((G28/1.5)*1000000,-5))/1000000</f>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C29" s="5">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D29" s="4">
+        <v>69</v>
+      </c>
+      <c r="E29" s="4">
         <v>65</v>
       </c>
-      <c r="E29" s="4">
-        <v>66</v>
-      </c>
       <c r="F29" s="4">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <f>ROUND(AVERAGE(D29:F29),1)</f>
+        <v>65.7</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="1"/>
-        <v>42.7</v>
+        <f>(ROUND((G29/1.5)*1000000,-5))/1000000</f>
+        <v>43.8</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4">
         <v>66</v>
       </c>
-      <c r="D30" s="4">
-        <v>68</v>
-      </c>
       <c r="E30" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="4">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="0"/>
-        <v>66</v>
+        <f>ROUND(AVERAGE(D30:F30),1)</f>
+        <v>65.7</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>(ROUND((G30/1.5)*1000000,-5))/1000000</f>
+        <v>43.8</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1278,40 +1323,45 @@
         <v>61</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(D31:F31),1)</f>
         <v>65.7</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="1"/>
+        <f>(ROUND((G31/1.5)*1000000,-5))/1000000</f>
         <v>43.8</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" s="5">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D32" s="4">
+        <v>65</v>
+      </c>
+      <c r="E32" s="4">
         <v>66</v>
       </c>
-      <c r="E32" s="4">
-        <v>69</v>
-      </c>
       <c r="F32" s="4">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="0"/>
-        <v>65.7</v>
+        <f>ROUND(AVERAGE(D32:F32),1)</f>
+        <v>64</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="1"/>
-        <v>43.8</v>
+        <f>(ROUND((G32/1.5)*1000000,-5))/1000000</f>
+        <v>42.7</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:H32">
+    <sortState ref="B3:H32">
+      <sortCondition descending="1" ref="G2:G32"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed driver salaries to make it more realistic (so you cannot buy 2 proffesional drivers from the start since you won't have enough money to buy upgrades etc.
</commit_message>
<xml_diff>
--- a/Docs/DriverStats.xlsx
+++ b/Docs/DriverStats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\A2B-Project\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$B$2:$H$32</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -140,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -288,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,26 +316,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,23 +351,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -569,7 +530,7 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,12 +584,12 @@
         <v>96</v>
       </c>
       <c r="G3" s="4">
-        <f>ROUND(AVERAGE(D3:F3),1)</f>
+        <f t="shared" ref="G3:G32" si="0">ROUND(AVERAGE(D3:F3),1)</f>
         <v>96</v>
       </c>
       <c r="H3" s="4">
-        <f>(ROUND((G3/1.5)*1000000,-5))/1000000</f>
-        <v>64</v>
+        <f>(ROUND((G3/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>84.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -648,12 +609,12 @@
         <v>93</v>
       </c>
       <c r="G4" s="4">
-        <f>ROUND(AVERAGE(D4:F4),1)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="H4" s="4">
-        <f>(ROUND((G4/1.5)*1000000,-5))/1000000</f>
-        <v>63.3</v>
+        <f t="shared" ref="H4:H32" si="1">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>83.6</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -673,12 +634,12 @@
         <v>95</v>
       </c>
       <c r="G5" s="4">
-        <f>ROUND(AVERAGE(D5:F5),1)</f>
+        <f t="shared" si="0"/>
         <v>94.7</v>
       </c>
       <c r="H5" s="4">
-        <f>(ROUND((G5/1.5)*1000000,-5))/1000000</f>
-        <v>63.1</v>
+        <f t="shared" si="1"/>
+        <v>83.3</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -698,12 +659,12 @@
         <v>94</v>
       </c>
       <c r="G6" s="4">
-        <f>ROUND(AVERAGE(D6:F6),1)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="H6" s="4">
-        <f>(ROUND((G6/1.5)*1000000,-5))/1000000</f>
-        <v>62.7</v>
+        <f t="shared" si="1"/>
+        <v>82.7</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -723,12 +684,12 @@
         <v>90</v>
       </c>
       <c r="G7" s="4">
-        <f>ROUND(AVERAGE(D7:F7),1)</f>
+        <f t="shared" si="0"/>
         <v>92.3</v>
       </c>
       <c r="H7" s="4">
-        <f>(ROUND((G7/1.5)*1000000,-5))/1000000</f>
-        <v>61.5</v>
+        <f t="shared" si="1"/>
+        <v>81.2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -748,12 +709,12 @@
         <v>90</v>
       </c>
       <c r="G8" s="4">
-        <f>ROUND(AVERAGE(D8:F8),1)</f>
+        <f t="shared" si="0"/>
         <v>90.7</v>
       </c>
       <c r="H8" s="4">
-        <f>(ROUND((G8/1.5)*1000000,-5))/1000000</f>
-        <v>60.5</v>
+        <f t="shared" si="1"/>
+        <v>79.8</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -773,12 +734,12 @@
         <v>85</v>
       </c>
       <c r="G9" s="4">
-        <f>ROUND(AVERAGE(D9:F9),1)</f>
+        <f t="shared" si="0"/>
         <v>85.7</v>
       </c>
       <c r="H9" s="4">
-        <f>(ROUND((G9/1.5)*1000000,-5))/1000000</f>
-        <v>57.1</v>
+        <f t="shared" si="1"/>
+        <v>75.400000000000006</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -798,12 +759,12 @@
         <v>82</v>
       </c>
       <c r="G10" s="4">
-        <f>ROUND(AVERAGE(D10:F10),1)</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="H10" s="4">
-        <f>(ROUND((G10/1.5)*1000000,-5))/1000000</f>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>73.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -823,12 +784,12 @@
         <v>83</v>
       </c>
       <c r="G11" s="4">
-        <f>ROUND(AVERAGE(D11:F11),1)</f>
+        <f t="shared" si="0"/>
         <v>82.3</v>
       </c>
       <c r="H11" s="4">
-        <f>(ROUND((G11/1.5)*1000000,-5))/1000000</f>
-        <v>54.9</v>
+        <f t="shared" si="1"/>
+        <v>72.400000000000006</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -848,12 +809,12 @@
         <v>82</v>
       </c>
       <c r="G12" s="4">
-        <f>ROUND(AVERAGE(D12:F12),1)</f>
+        <f t="shared" si="0"/>
         <v>79.7</v>
       </c>
       <c r="H12" s="4">
-        <f>(ROUND((G12/1.5)*1000000,-5))/1000000</f>
-        <v>53.1</v>
+        <f t="shared" si="1"/>
+        <v>70.099999999999994</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -873,12 +834,12 @@
         <v>82</v>
       </c>
       <c r="G13" s="4">
-        <f>ROUND(AVERAGE(D13:F13),1)</f>
+        <f t="shared" si="0"/>
         <v>78.7</v>
       </c>
       <c r="H13" s="4">
-        <f>(ROUND((G13/1.5)*1000000,-5))/1000000</f>
-        <v>52.5</v>
+        <f t="shared" si="1"/>
+        <v>69.3</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -898,12 +859,12 @@
         <v>78</v>
       </c>
       <c r="G14" s="4">
-        <f>ROUND(AVERAGE(D14:F14),1)</f>
+        <f t="shared" si="0"/>
         <v>78.7</v>
       </c>
       <c r="H14" s="4">
-        <f>(ROUND((G14/1.5)*1000000,-5))/1000000</f>
-        <v>52.5</v>
+        <f t="shared" si="1"/>
+        <v>69.3</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -923,12 +884,12 @@
         <v>75</v>
       </c>
       <c r="G15" s="4">
-        <f>ROUND(AVERAGE(D15:F15),1)</f>
+        <f t="shared" si="0"/>
         <v>77.3</v>
       </c>
       <c r="H15" s="4">
-        <f>(ROUND((G15/1.5)*1000000,-5))/1000000</f>
-        <v>51.5</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -948,12 +909,12 @@
         <v>80</v>
       </c>
       <c r="G16" s="4">
-        <f>ROUND(AVERAGE(D16:F16),1)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="H16" s="4">
-        <f>(ROUND((G16/1.5)*1000000,-5))/1000000</f>
-        <v>51.3</v>
+        <f t="shared" si="1"/>
+        <v>67.8</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -973,12 +934,12 @@
         <v>79</v>
       </c>
       <c r="G17" s="4">
-        <f>ROUND(AVERAGE(D17:F17),1)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="H17" s="4">
-        <f>(ROUND((G17/1.5)*1000000,-5))/1000000</f>
-        <v>51.3</v>
+        <f t="shared" si="1"/>
+        <v>67.8</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -998,12 +959,12 @@
         <v>75</v>
       </c>
       <c r="G18" s="4">
-        <f>ROUND(AVERAGE(D18:F18),1)</f>
+        <f t="shared" si="0"/>
         <v>76.7</v>
       </c>
       <c r="H18" s="4">
-        <f>(ROUND((G18/1.5)*1000000,-5))/1000000</f>
-        <v>51.1</v>
+        <f t="shared" si="1"/>
+        <v>67.5</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1023,12 +984,12 @@
         <v>74</v>
       </c>
       <c r="G19" s="4">
-        <f>ROUND(AVERAGE(D19:F19),1)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="H19" s="4">
-        <f>(ROUND((G19/1.5)*1000000,-5))/1000000</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1048,12 +1009,12 @@
         <v>71</v>
       </c>
       <c r="G20" s="4">
-        <f>ROUND(AVERAGE(D20:F20),1)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="H20" s="4">
-        <f>(ROUND((G20/1.5)*1000000,-5))/1000000</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1073,12 +1034,12 @@
         <v>74</v>
       </c>
       <c r="G21" s="4">
-        <f>ROUND(AVERAGE(D21:F21),1)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="H21" s="4">
-        <f>(ROUND((G21/1.5)*1000000,-5))/1000000</f>
-        <v>49.3</v>
+        <f t="shared" si="1"/>
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1098,12 +1059,12 @@
         <v>71</v>
       </c>
       <c r="G22" s="4">
-        <f>ROUND(AVERAGE(D22:F22),1)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="H22" s="4">
-        <f>(ROUND((G22/1.5)*1000000,-5))/1000000</f>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>63.4</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1123,12 +1084,12 @@
         <v>72</v>
       </c>
       <c r="G23" s="4">
-        <f>ROUND(AVERAGE(D23:F23),1)</f>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="H23" s="4">
-        <f>(ROUND((G23/1.5)*1000000,-5))/1000000</f>
-        <v>47.3</v>
+        <f t="shared" si="1"/>
+        <v>62.5</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1148,12 +1109,12 @@
         <v>69</v>
       </c>
       <c r="G24" s="4">
-        <f>ROUND(AVERAGE(D24:F24),1)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="H24" s="4">
-        <f>(ROUND((G24/1.5)*1000000,-5))/1000000</f>
-        <v>46.7</v>
+        <f t="shared" si="1"/>
+        <v>61.6</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1173,12 +1134,12 @@
         <v>66</v>
       </c>
       <c r="G25" s="4">
-        <f>ROUND(AVERAGE(D25:F25),1)</f>
+        <f t="shared" si="0"/>
         <v>69.3</v>
       </c>
       <c r="H25" s="4">
-        <f>(ROUND((G25/1.5)*1000000,-5))/1000000</f>
-        <v>46.2</v>
+        <f t="shared" si="1"/>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1198,12 +1159,12 @@
         <v>65</v>
       </c>
       <c r="G26" s="4">
-        <f>ROUND(AVERAGE(D26:F26),1)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="H26" s="4">
-        <f>(ROUND((G26/1.5)*1000000,-5))/1000000</f>
-        <v>45.3</v>
+        <f t="shared" si="1"/>
+        <v>59.8</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1223,12 +1184,12 @@
         <v>64</v>
       </c>
       <c r="G27" s="4">
-        <f>ROUND(AVERAGE(D27:F27),1)</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="H27" s="4">
-        <f>(ROUND((G27/1.5)*1000000,-5))/1000000</f>
-        <v>44.7</v>
+        <f t="shared" si="1"/>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1248,12 +1209,12 @@
         <v>60</v>
       </c>
       <c r="G28" s="4">
-        <f>ROUND(AVERAGE(D28:F28),1)</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="H28" s="4">
-        <f>(ROUND((G28/1.5)*1000000,-5))/1000000</f>
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>58.1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1273,12 +1234,12 @@
         <v>63</v>
       </c>
       <c r="G29" s="4">
-        <f>ROUND(AVERAGE(D29:F29),1)</f>
+        <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
       <c r="H29" s="4">
-        <f>(ROUND((G29/1.5)*1000000,-5))/1000000</f>
-        <v>43.8</v>
+        <f t="shared" si="1"/>
+        <v>57.8</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1298,12 +1259,12 @@
         <v>62</v>
       </c>
       <c r="G30" s="4">
-        <f>ROUND(AVERAGE(D30:F30),1)</f>
+        <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
       <c r="H30" s="4">
-        <f>(ROUND((G30/1.5)*1000000,-5))/1000000</f>
-        <v>43.8</v>
+        <f t="shared" si="1"/>
+        <v>57.8</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1323,12 +1284,12 @@
         <v>61</v>
       </c>
       <c r="G31" s="4">
-        <f>ROUND(AVERAGE(D31:F31),1)</f>
+        <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
       <c r="H31" s="4">
-        <f>(ROUND((G31/1.5)*1000000,-5))/1000000</f>
-        <v>43.8</v>
+        <f t="shared" si="1"/>
+        <v>57.8</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1348,12 +1309,12 @@
         <v>61</v>
       </c>
       <c r="G32" s="4">
-        <f>ROUND(AVERAGE(D32:F32),1)</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="H32" s="4">
-        <f>(ROUND((G32/1.5)*1000000,-5))/1000000</f>
-        <v>42.7</v>
+        <f t="shared" si="1"/>
+        <v>56.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>